<commit_message>
minor change to stations json
</commit_message>
<xml_diff>
--- a/src/main/resources/com/metro/prediction/metroroutepredictor/Modified_DMRC_Stations.xlsx
+++ b/src/main/resources/com/metro/prediction/metroroutepredictor/Modified_DMRC_Stations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikas\IdeaProjects\MetroRoutePredictor\src\main\resources\com\metro\prediction\metroroutepredictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87A8EAA-1658-4653-AE33-3DDB1CC471D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23B9386-05C9-4423-8F0B-52F3007A88A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1824" yWindow="1800" windowWidth="17280" windowHeight="9420" xr2:uid="{F6A641C7-A60E-4E32-B5C5-1DBCE25BBE34}"/>
+    <workbookView xWindow="2172" yWindow="2148" windowWidth="17280" windowHeight="9420" xr2:uid="{F6A641C7-A60E-4E32-B5C5-1DBCE25BBE34}"/>
   </bookViews>
   <sheets>
     <sheet name="Lines" sheetId="1" r:id="rId1"/>
@@ -962,13 +962,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:H289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1303,16 +1303,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1321,18 +1321,19 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
@@ -6992,36 +6993,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A32"/>
+    <mergeCell ref="B4:B32"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="A33:A69"/>
+    <mergeCell ref="B33:B69"/>
+    <mergeCell ref="A70:A119"/>
+    <mergeCell ref="B70:B119"/>
+    <mergeCell ref="A120:A125"/>
+    <mergeCell ref="B120:B125"/>
+    <mergeCell ref="A126:A146"/>
+    <mergeCell ref="B126:B146"/>
+    <mergeCell ref="A147:A157"/>
+    <mergeCell ref="B147:B157"/>
+    <mergeCell ref="A158:A191"/>
+    <mergeCell ref="B158:B191"/>
+    <mergeCell ref="A192:A216"/>
+    <mergeCell ref="B192:B216"/>
+    <mergeCell ref="A217:A254"/>
+    <mergeCell ref="B217:B254"/>
+    <mergeCell ref="A255:A262"/>
+    <mergeCell ref="B255:B262"/>
     <mergeCell ref="A263:A265"/>
     <mergeCell ref="B263:B265"/>
     <mergeCell ref="A266:A286"/>
     <mergeCell ref="B266:B286"/>
     <mergeCell ref="A287:A289"/>
     <mergeCell ref="B287:B289"/>
-    <mergeCell ref="A192:A216"/>
-    <mergeCell ref="B192:B216"/>
-    <mergeCell ref="A217:A254"/>
-    <mergeCell ref="B217:B254"/>
-    <mergeCell ref="A255:A262"/>
-    <mergeCell ref="B255:B262"/>
-    <mergeCell ref="A126:A146"/>
-    <mergeCell ref="B126:B146"/>
-    <mergeCell ref="A147:A157"/>
-    <mergeCell ref="B147:B157"/>
-    <mergeCell ref="A158:A191"/>
-    <mergeCell ref="B158:B191"/>
-    <mergeCell ref="A33:A69"/>
-    <mergeCell ref="B33:B69"/>
-    <mergeCell ref="A70:A119"/>
-    <mergeCell ref="B70:B119"/>
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="B120:B125"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="A4:A32"/>
-    <mergeCell ref="B4:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>